<commit_message>
git config --global user.email "phuongtdv@gmail.com"
</commit_message>
<xml_diff>
--- a/SNMP_Project_ChangesNote_R01.xlsx
+++ b/SNMP_Project_ChangesNote_R01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phuongtdv\Dropbox\ADCT\00_SNMPFPT\01_Requirement\PIF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Phuong\Git\PhuongTDVTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16700"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="8" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
   <si>
     <t>Owner</t>
   </si>
@@ -152,9 +152,6 @@
     <t>Add 1 RS485 connector</t>
   </si>
   <si>
-    <t>Changed 6 small relays to Solid state relay if possible (design/BoM/price suggestion first)</t>
-  </si>
-  <si>
     <t>Suggest connector e.g. power connector from power board, 1wire, rs485/232 if it's better</t>
   </si>
   <si>
@@ -201,9 +198,6 @@
     <t>Project Plan'!B11</t>
   </si>
   <si>
-    <t>RS422 connection is timed out randomly (some board have 1, 2 message before timed out; some 10, 20; some 100, 200…)</t>
-  </si>
-  <si>
     <t>Highest</t>
   </si>
   <si>
@@ -214,9 +208,6 @@
   </si>
   <si>
     <t>Project Plan'!B14</t>
-  </si>
-  <si>
-    <t>All input/output should be placed according to Vu's 3D design. Suggestions are welcome as well.</t>
   </si>
   <si>
     <r>
@@ -249,6 +240,70 @@
         <family val="1"/>
       </rPr>
       <t>[08Apr] Cái SSR này phụ thuộc vào lại tải nữa hả Phương? Tại anh tính làm nó universal và có thể áp dụng được cho SmartOutlet (đóng mở nguồn các thiết bị điện trong nhà: đèn, quạt, máy lạnh...)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Changed 6 small relays to Solid state relay if possible (design/BoM/price suggestion first)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NC when power is cut off or the device is shutted down
+AC outputs: 220VAC/5kW
+6 DC outputs: 48VDC/100W</t>
+    </r>
+  </si>
+  <si>
+    <t>Power connector should be improved to:
+1. In Tri Viet board - 48VDC input connector: http://thegioiic.com/products/hb9500-2p
+2. In Tri Viet board - 12V/5V output connector:
+http://thegioiic.com/products/5557-power-connector-wire
+3. In Relay board - 12V/5V input connector:
+Same as No.2</t>
+  </si>
+  <si>
+    <t>Reverse engineer Tri Viet power board if possible and cheaper than buying from Tri Viet. Pulse transformer can be bought from Tri Viet.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All input/output should be placed according to Vu's 3D design. Suggestions are welcome as well.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>If possible, Tri Viet power board should be placed in the same surface as relay board.</t>
+    </r>
+  </si>
+  <si>
+    <t>Add 2 connectors: 12V and 5V output (for external sensor usage) to Relay board (near the inputs of Burglar, Fire, Smoke, Water…)</t>
+  </si>
+  <si>
+    <t>Review RS422 board to see if connection time</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">RS422 connection is timed out randomly (some board have 1, 2 message before timed out; some 10, 20; some 100, 200…).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Review RS422 board and RS422 in Main board is needed to see if the connection time out is caused by hardware.</t>
     </r>
   </si>
 </sst>
@@ -412,7 +467,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -452,12 +507,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -507,6 +556,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -803,7 +861,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -838,7 +896,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1025,320 +1083,336 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.4609375" style="32" customWidth="1"/>
-    <col min="2" max="2" width="9.23046875" style="32"/>
-    <col min="3" max="3" width="55.61328125" style="33" customWidth="1"/>
-    <col min="4" max="4" width="12.61328125" style="32" customWidth="1"/>
-    <col min="5" max="5" width="9.23046875" style="32"/>
-    <col min="6" max="6" width="17.23046875" style="32" customWidth="1"/>
-    <col min="7" max="16384" width="9.23046875" style="32"/>
+    <col min="1" max="1" width="1.4609375" style="30" customWidth="1"/>
+    <col min="2" max="2" width="9.23046875" style="30"/>
+    <col min="3" max="3" width="55.61328125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="12.61328125" style="30" customWidth="1"/>
+    <col min="5" max="5" width="9.23046875" style="30"/>
+    <col min="6" max="6" width="17.23046875" style="30" customWidth="1"/>
+    <col min="7" max="16384" width="9.23046875" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="8.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="33" x14ac:dyDescent="0.35">
+      <c r="B3" s="27">
+        <v>1</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E3" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="27"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="27">
+        <v>2</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="27">
+        <v>3</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="66" x14ac:dyDescent="0.35">
+      <c r="B6" s="27">
+        <v>4</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="27"/>
+    </row>
+    <row r="7" spans="2:6" ht="82.5" x14ac:dyDescent="0.35">
+      <c r="B7" s="27">
+        <v>5</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="33" x14ac:dyDescent="0.35">
+      <c r="B8" s="27">
+        <v>6</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="27"/>
+    </row>
+    <row r="9" spans="2:6" ht="66" x14ac:dyDescent="0.35">
+      <c r="B9" s="27">
+        <v>7</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="34" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="33" x14ac:dyDescent="0.35">
-      <c r="B3" s="29">
-        <v>1</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="29" t="s">
+      <c r="E9" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="27"/>
+    </row>
+    <row r="10" spans="2:6" ht="115.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="27">
+        <v>8</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E10" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="27"/>
+    </row>
+    <row r="11" spans="2:6" ht="49.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="27">
+        <v>9</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+    </row>
+    <row r="12" spans="2:6" ht="33" x14ac:dyDescent="0.35">
+      <c r="B12" s="27">
+        <v>10</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="29"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="29">
-        <v>2</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="29">
-        <v>3</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="33" x14ac:dyDescent="0.35">
-      <c r="B6" s="29">
-        <v>4</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="29"/>
-    </row>
-    <row r="7" spans="2:6" ht="33" x14ac:dyDescent="0.35">
-      <c r="B7" s="29">
-        <v>5</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="33" x14ac:dyDescent="0.35">
-      <c r="B8" s="29">
-        <v>6</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="29"/>
-    </row>
-    <row r="9" spans="2:6" ht="33" x14ac:dyDescent="0.35">
-      <c r="B9" s="29">
-        <v>7</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="29"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="29">
-        <v>8</v>
-      </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="29">
-        <v>9</v>
-      </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="29">
-        <v>10</v>
-      </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="F12" s="27"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="29">
+      <c r="B13" s="27">
         <v>11</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
+      <c r="C13" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="29">
+      <c r="B14" s="27">
         <v>12</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B15" s="29"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="29"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="29"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="29"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="29"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="29"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="29"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B25" s="29"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="29"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="29"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="29"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B29" s="29"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B30" s="29"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B31" s="29"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B32" s="29"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1352,6 +1426,7 @@
     <hyperlink ref="F7" location="'Project Plan'!B14" display="Project Plan'!B14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1371,7 +1446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1390,18 +1465,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="15" t="s">
+      <c r="A1" s="35"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1416,8 +1491,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1455,263 +1530,263 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="66" x14ac:dyDescent="0.35">
-      <c r="A7" s="19">
+    <row r="7" spans="1:9" ht="49.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="17">
         <v>42464</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="18">
         <v>1</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="22"/>
-    </row>
-    <row r="8" spans="1:9" ht="82.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="24">
+      <c r="E7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:9" ht="49.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="22">
         <v>42464</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="23">
         <v>2</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="28"/>
-    </row>
-    <row r="9" spans="1:9" ht="49.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="19">
+      <c r="E8" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="26"/>
+    </row>
+    <row r="9" spans="1:9" ht="33" x14ac:dyDescent="0.35">
+      <c r="A9" s="17">
         <v>42464</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="18">
         <v>3</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="22"/>
+      <c r="E9" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="24">
+      <c r="A10" s="22">
         <v>42464</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="23">
         <v>4</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="27" t="s">
+      <c r="E10" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="25" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="19">
+      <c r="A11" s="17">
         <v>42464</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="18">
         <v>5</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="22" t="s">
+      <c r="E11" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="20" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="99" x14ac:dyDescent="0.35">
-      <c r="A12" s="24">
+      <c r="A12" s="22">
         <v>42465</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="23">
         <v>6</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="27" t="s">
+      <c r="D12" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="66" x14ac:dyDescent="0.35">
-      <c r="A13" s="19">
+    <row r="13" spans="1:9" ht="49.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="17">
         <v>42465</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="18">
         <v>7</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="22"/>
+      <c r="E13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:9" ht="132" x14ac:dyDescent="0.35">
-      <c r="A14" s="24">
+      <c r="A14" s="22">
         <v>42465</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="23">
         <v>8</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="27" t="s">
+      <c r="D14" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="49.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="19">
+    <row r="15" spans="1:9" ht="33" x14ac:dyDescent="0.35">
+      <c r="A15" s="17">
         <v>42466</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15" s="18">
         <v>9</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="22" t="s">
+      <c r="E15" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="24">
+      <c r="A16" s="22">
         <v>42466</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="23">
         <v>10</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="27"/>
+      <c r="E16" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="25"/>
     </row>
     <row r="17" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="19">
+      <c r="A17" s="17">
         <v>42466</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B17" s="18">
         <v>11</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="49.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="24">
+    <row r="18" spans="1:6" ht="33" x14ac:dyDescent="0.35">
+      <c r="A18" s="22">
         <v>42466</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="23">
         <v>12</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="27" t="s">
+      <c r="E18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="22"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="28"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="26"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="22"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="20"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="28"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="26"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B23" s="3"/>
@@ -2135,7 +2210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -2161,36 +2236,36 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" t="s">
         <v>55</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>